<commit_message>
All tests pass. Need to make Compiler tests and update UI.
</commit_message>
<xml_diff>
--- a/doc-engine-core/src/test/resources/test-data-read.xlsx
+++ b/doc-engine-core/src/test/resources/test-data-read.xlsx
@@ -25,9 +25,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Boolean Test</t>
-  </si>
-  <si>
     <t>TEST Name - 0</t>
   </si>
   <si>
@@ -626,6 +623,9 @@
   </si>
   <si>
     <t>TEST Description - 99</t>
+  </si>
+  <si>
+    <t>Positive</t>
   </si>
 </sst>
 </file>
@@ -960,7 +960,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,7 +982,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -990,10 +990,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1004,10 +1004,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1018,10 +1018,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1032,10 +1032,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1046,10 +1046,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1060,10 +1060,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -1074,10 +1074,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -1088,10 +1088,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1102,10 +1102,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1116,10 +1116,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -1130,10 +1130,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1144,10 +1144,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1158,10 +1158,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1172,10 +1172,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -1186,10 +1186,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1200,10 +1200,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1214,10 +1214,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1228,10 +1228,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1242,10 +1242,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1256,10 +1256,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1270,10 +1270,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1284,10 +1284,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -1298,10 +1298,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" t="s">
-        <v>49</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1312,10 +1312,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1326,10 +1326,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -1340,10 +1340,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1354,10 +1354,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1368,10 +1368,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1382,10 +1382,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -1396,10 +1396,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -1410,10 +1410,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" t="s">
-        <v>65</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -1424,10 +1424,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1438,10 +1438,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -1452,10 +1452,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1466,10 +1466,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1480,10 +1480,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
         <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -1494,10 +1494,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
         <v>76</v>
-      </c>
-      <c r="C38" t="s">
-        <v>77</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1508,10 +1508,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1522,10 +1522,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
         <v>80</v>
-      </c>
-      <c r="C40" t="s">
-        <v>81</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1536,10 +1536,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1550,10 +1550,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -1564,10 +1564,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
         <v>86</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -1578,10 +1578,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
         <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1592,10 +1592,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -1606,10 +1606,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
         <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1620,10 +1620,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
         <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>95</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -1634,10 +1634,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
         <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -1648,10 +1648,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
         <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1662,10 +1662,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
         <v>100</v>
-      </c>
-      <c r="C50" t="s">
-        <v>101</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -1676,10 +1676,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
         <v>102</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -1690,10 +1690,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
         <v>104</v>
-      </c>
-      <c r="C52" t="s">
-        <v>105</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -1704,10 +1704,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
         <v>106</v>
-      </c>
-      <c r="C53" t="s">
-        <v>107</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -1718,10 +1718,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
         <v>108</v>
-      </c>
-      <c r="C54" t="s">
-        <v>109</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -1732,10 +1732,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
         <v>110</v>
-      </c>
-      <c r="C55" t="s">
-        <v>111</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -1746,10 +1746,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" t="s">
         <v>112</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -1760,10 +1760,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
         <v>114</v>
-      </c>
-      <c r="C57" t="s">
-        <v>115</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -1774,10 +1774,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
         <v>116</v>
-      </c>
-      <c r="C58" t="s">
-        <v>117</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -1788,10 +1788,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s">
         <v>118</v>
-      </c>
-      <c r="C59" t="s">
-        <v>119</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -1802,10 +1802,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
         <v>120</v>
-      </c>
-      <c r="C60" t="s">
-        <v>121</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -1816,10 +1816,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
         <v>122</v>
-      </c>
-      <c r="C61" t="s">
-        <v>123</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -1830,10 +1830,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
         <v>124</v>
-      </c>
-      <c r="C62" t="s">
-        <v>125</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -1844,10 +1844,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
         <v>126</v>
-      </c>
-      <c r="C63" t="s">
-        <v>127</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -1858,10 +1858,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>129</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -1872,10 +1872,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
         <v>130</v>
-      </c>
-      <c r="C65" t="s">
-        <v>131</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -1886,10 +1886,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
         <v>132</v>
-      </c>
-      <c r="C66" t="s">
-        <v>133</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -1900,10 +1900,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
         <v>134</v>
-      </c>
-      <c r="C67" t="s">
-        <v>135</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -1914,10 +1914,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" t="s">
         <v>136</v>
-      </c>
-      <c r="C68" t="s">
-        <v>137</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -1928,10 +1928,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" t="s">
         <v>138</v>
-      </c>
-      <c r="C69" t="s">
-        <v>139</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -1942,10 +1942,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" t="s">
         <v>140</v>
-      </c>
-      <c r="C70" t="s">
-        <v>141</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -1956,10 +1956,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" t="s">
         <v>142</v>
-      </c>
-      <c r="C71" t="s">
-        <v>143</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -1970,10 +1970,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" t="s">
         <v>144</v>
-      </c>
-      <c r="C72" t="s">
-        <v>145</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -1984,10 +1984,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" t="s">
         <v>146</v>
-      </c>
-      <c r="C73" t="s">
-        <v>147</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -1998,10 +1998,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" t="s">
         <v>148</v>
-      </c>
-      <c r="C74" t="s">
-        <v>149</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -2012,10 +2012,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" t="s">
         <v>150</v>
-      </c>
-      <c r="C75" t="s">
-        <v>151</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -2026,10 +2026,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="s">
         <v>152</v>
-      </c>
-      <c r="C76" t="s">
-        <v>153</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -2040,10 +2040,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" t="s">
         <v>154</v>
-      </c>
-      <c r="C77" t="s">
-        <v>155</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -2054,10 +2054,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" t="s">
         <v>156</v>
-      </c>
-      <c r="C78" t="s">
-        <v>157</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -2068,10 +2068,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" t="s">
         <v>158</v>
-      </c>
-      <c r="C79" t="s">
-        <v>159</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -2082,10 +2082,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" t="s">
         <v>160</v>
-      </c>
-      <c r="C80" t="s">
-        <v>161</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -2096,10 +2096,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" t="s">
         <v>162</v>
-      </c>
-      <c r="C81" t="s">
-        <v>163</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -2110,10 +2110,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" t="s">
         <v>164</v>
-      </c>
-      <c r="C82" t="s">
-        <v>165</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -2124,10 +2124,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" t="s">
         <v>166</v>
-      </c>
-      <c r="C83" t="s">
-        <v>167</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -2138,10 +2138,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84" t="s">
         <v>168</v>
-      </c>
-      <c r="C84" t="s">
-        <v>169</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -2152,10 +2152,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>169</v>
+      </c>
+      <c r="C85" t="s">
         <v>170</v>
-      </c>
-      <c r="C85" t="s">
-        <v>171</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -2166,10 +2166,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" t="s">
         <v>172</v>
-      </c>
-      <c r="C86" t="s">
-        <v>173</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -2180,10 +2180,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" t="s">
         <v>174</v>
-      </c>
-      <c r="C87" t="s">
-        <v>175</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -2194,10 +2194,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" t="s">
         <v>176</v>
-      </c>
-      <c r="C88" t="s">
-        <v>177</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -2208,10 +2208,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" t="s">
         <v>178</v>
-      </c>
-      <c r="C89" t="s">
-        <v>179</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -2222,10 +2222,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
+        <v>179</v>
+      </c>
+      <c r="C90" t="s">
         <v>180</v>
-      </c>
-      <c r="C90" t="s">
-        <v>181</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -2236,10 +2236,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" t="s">
         <v>182</v>
-      </c>
-      <c r="C91" t="s">
-        <v>183</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -2250,10 +2250,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" t="s">
         <v>184</v>
-      </c>
-      <c r="C92" t="s">
-        <v>185</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -2264,10 +2264,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
+        <v>185</v>
+      </c>
+      <c r="C93" t="s">
         <v>186</v>
-      </c>
-      <c r="C93" t="s">
-        <v>187</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -2278,10 +2278,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
+        <v>187</v>
+      </c>
+      <c r="C94" t="s">
         <v>188</v>
-      </c>
-      <c r="C94" t="s">
-        <v>189</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -2292,10 +2292,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
+        <v>189</v>
+      </c>
+      <c r="C95" t="s">
         <v>190</v>
-      </c>
-      <c r="C95" t="s">
-        <v>191</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -2306,10 +2306,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" t="s">
         <v>192</v>
-      </c>
-      <c r="C96" t="s">
-        <v>193</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -2320,10 +2320,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" t="s">
         <v>194</v>
-      </c>
-      <c r="C97" t="s">
-        <v>195</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -2334,10 +2334,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" t="s">
         <v>196</v>
-      </c>
-      <c r="C98" t="s">
-        <v>197</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -2348,10 +2348,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" t="s">
         <v>198</v>
-      </c>
-      <c r="C99" t="s">
-        <v>199</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -2362,10 +2362,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>199</v>
+      </c>
+      <c r="C100" t="s">
         <v>200</v>
-      </c>
-      <c r="C100" t="s">
-        <v>201</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -2376,10 +2376,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" t="s">
         <v>202</v>
-      </c>
-      <c r="C101" t="s">
-        <v>203</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>

</xml_diff>